<commit_message>
Add updated notebooks and classification results, new interest rate data
</commit_message>
<xml_diff>
--- a/OpenAI Classification/classified_articles.xlsx
+++ b/OpenAI Classification/classified_articles.xlsx
@@ -503,7 +503,7 @@
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>The article suggests a hawkish sentiment as it highlights the Governing Council's determination to ensure inflation returns to its 2% target and mentions the need for interest rates to stay sufficiently restrictive. This indicates a leaning towards combating inflation and potentially tightening monetary policy.</t>
+          <t>The article suggests a hawkish tone as it emphasizes the need to combat inflation and return it to the 2% target. It highlights that inflation is being pushed down due to restrictive financing conditions and past interest rate increases. Additionally, the Governing Council mentions the possibility of reducing monetary policy restriction if confident in inflation convergence but also states it will continue to follow a data-dependent approach. Overall, the strong focus on price stability and willingness to adjust instruments to achieve the inflation target leans towards a hawkish stance.</t>
         </is>
       </c>
     </row>
@@ -535,12 +535,12 @@
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>0.8</t>
+          <t>0.6</t>
         </is>
       </c>
       <c r="G3" t="inlineStr">
         <is>
-          <t>The article suggests a hawkish sentiment as the ECB is concerned about low inflation rates and aims to return inflation to its 2% target. The Governing Council states that they will continue to set interest rates at restrictive levels for as long as necessary to combat low inflation. Additionally, they mention that they are ready to adjust all instruments within their mandate to ensure the return of inflation to the 2% target over the medium term. The emphasis on maintaining restrictive interest rates and adjusting policies to combat low inflation signals a hawkish stance.</t>
+          <t>The article indicates a hawkish stance as the ECB is focused on combating low inflation by maintaining restrictive policy rates for as long as necessary. The projections show a downward revision in inflation rates, with the Governing Council determined to ensure inflation returns to its 2% target. The emphasis on maintaining restrictive interest rates and reducing the PEPP portfolio suggests a hawkish sentiment towards monetary policy.</t>
         </is>
       </c>
     </row>
@@ -577,7 +577,7 @@
       </c>
       <c r="G4" t="inlineStr">
         <is>
-          <t>The article suggests a hawkish stance by indicating that the Governing Council is determined to ensure inflation returns to its 2% target and that current interest rates are viewed as sufficiently restrictive. The emphasis on maintaining restrictive levels for as long as necessary and adjusting all instruments within its mandate to combat inflation signals a hawkish sentiment.</t>
+          <t>The article suggests a hawkish stance as it emphasizes the Governing Council's determination to ensure that inflation returns to its 2% medium-term target in a timely manner by maintaining interest rates at restrictive levels. It highlights the impact of tight financing conditions on dampening demand and pushing down inflation, indicating a bias towards combating inflation rather than supporting economic growth.</t>
         </is>
       </c>
     </row>
@@ -614,7 +614,7 @@
       </c>
       <c r="G5" t="inlineStr">
         <is>
-          <t>The article suggests a hawkish stance as it highlights concerns about elevated inflation and the determination of the Governing Council to ensure inflation returns to its 2% target in a timely manner. The mention of maintaining interest rates at restrictive levels to contribute to this goal also supports a hawkish view on monetary policy.</t>
+          <t>The article suggests a hawkish sentiment by emphasizing the Governing Council's determination to ensure inflation returns to the 2% target, maintaining interest rates at restrictive levels for as long as necessary, and advancing the normalisation of the balance sheet. The downward revision of inflation projections for 2023 and 2024, coupled with the focus on combating inflation and tightening monetary policy, contribute to the hawkish classification and score.</t>
         </is>
       </c>
     </row>
@@ -651,7 +651,7 @@
       </c>
       <c r="G6" t="inlineStr">
         <is>
-          <t>The article indicates a hawkish stance as it emphasizes the need to combat inflation and return it to the 2% target. The Governing Council is committed to maintaining interest rates at restrictive levels for as long as necessary and stands ready to adjust all instruments to achieve its inflation goal. This suggests a strong inclination towards monetary tightening and a hawkish bias to the overall policy stance.</t>
+          <t>The article suggests a hawkish stance by indicating that inflation is expected to stay high, domestic price pressures are strong, and past interest rate increases are dampening demand to help push down inflation. The Governing Council is determined to ensure inflation returns to its 2% target, and future decisions will ensure that policy rates will be set at restrictive levels for as long as necessary. The emphasis on maintaining interest rates at levels that will contribute to reducing inflation and the readiness to adjust all instruments within the mandate to achieve the 2% target indicate a hawkish sentiment.</t>
         </is>
       </c>
     </row>
@@ -683,12 +683,12 @@
       </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t>0.8</t>
+          <t>0.9</t>
         </is>
       </c>
       <c r="G7" t="inlineStr">
         <is>
-          <t>The article suggests a hawkish stance by stating the central bank's determination to combat high inflation and raise interest rates to achieve its 2% target. The upward revisions in inflation projections, the tightening of financing conditions, and the emphasis on maintaining restrictive interest rate levels contribute to the hawkish tone of the article.</t>
+          <t>The article suggests a hawkish stance by highlighting the increase in ECB interest rates in response to high inflation and tightening financing conditions. The Governing Council is determined to combat inflation and bring it back to the 2% target. This indicates a prioritization of controlling inflation over supporting economic growth, which is a hawkish approach.</t>
         </is>
       </c>
     </row>
@@ -725,7 +725,7 @@
       </c>
       <c r="G8" t="inlineStr">
         <is>
-          <t>The article suggests a hawkish stance as it highlights the determination to combat inflation and raise interest rates to achieve the 2% inflation target. The emphasis on restrictive monetary policy, tightening financing conditions, and raising key ECB interest rates indicates a hawkish approach. The focus on managing inflation expectations through policy adjustments and ensuring effective transmission of monetary policy further supports the hawkish classification.</t>
+          <t>The article suggests a hawkish stance as the ECB has decided to raise the key interest rates by 25 basis points in order to combat inflation and bring it back to the 2% target. The language used in the article emphasizes the need for restrictive monetary policy for an extended period to achieve the inflation target, indicating a hawkish tone.</t>
         </is>
       </c>
     </row>
@@ -757,12 +757,12 @@
       </c>
       <c r="F9" t="inlineStr">
         <is>
-          <t>0.8</t>
+          <t>0.7</t>
         </is>
       </c>
       <c r="G9" t="inlineStr">
         <is>
-          <t>The article indicates a hawkish stance by stating the need to raise interest rates to combat high inflation and ensure a timely return to the 2% target. The emphasis on maintaining restrictive interest rates for as long as necessary, tightening financing conditions, and managing the asset purchase programs to avoid interference with monetary policy stance all point towards a hawkish policy approach. The score of 0.8 reflects a strong hawkish tone in the article.</t>
+          <t>The article suggests a hawkish stance as the Governing Council decided to raise interest rates due to concerns about high inflation levels. The language used emphasizes the need to combat inflation and achieve the 2% medium-term target, indicating a hawkish sentiment towards monetary policy.</t>
         </is>
       </c>
     </row>
@@ -799,7 +799,7 @@
       </c>
       <c r="G10" t="inlineStr">
         <is>
-          <t>The article indicates a hawkish stance as the ECB has decided to raise interest rates by 25 basis points to combat high inflation. The ECB's focus on achieving the 2% inflation target and the determination to bring inflation down to target levels through restrictive monetary policy measures signal a hawkish tone. The measures to discontinue reinvestments under the asset purchase programme and manage the PEPP portfolio also contribute to the hawkish outlook.</t>
+          <t>The article suggests hawkish sentiments as the European Central Bank (ECB) has decided to raise interest rates by 25 basis points to combat high inflation. The ECB aims to bring inflation back to its 2% target and indicates a willingness to implement restrictive policies as necessary to achieve this goal. This indicates a hawkish stance towards monetary policy.</t>
         </is>
       </c>
     </row>
@@ -826,17 +826,17 @@
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>Error</t>
+          <t>Hawkish</t>
         </is>
       </c>
       <c r="F11" t="inlineStr">
         <is>
-          <t>Error</t>
+          <t>0.8</t>
         </is>
       </c>
       <c r="G11" t="inlineStr">
         <is>
-          <t>Error</t>
+          <t>The article indicates a hawkish stance by highlighting concerns about high inflation and announcing a decision to raise interest rates in order to combat inflation and bring it back to the 2% target. The language used regarding future policy decisions and the emphasis on tightening monetary policy support the hawkish classification.</t>
         </is>
       </c>
     </row>
@@ -873,7 +873,7 @@
       </c>
       <c r="G12" t="inlineStr">
         <is>
-          <t>The article suggests a hawkish sentiment as the ECB decided to raise interest rates by 50 basis points to combat high inflation. The focus is on the importance of returning inflation to the 2% target and the role of tighter monetary policy in dampening demand and stabilizing prices. The measures taken indicate a stance more aligned with fighting inflation than supporting economic growth.</t>
+          <t>The article suggests a hawkish stance by indicating that the ECB has decided to increase interest rates to combat high inflation. It emphasizes the importance of returning inflation to the 2% target and mentions the tightening of monetary policy to dampen demand pressures. Additionally, the article discusses resilience in the banking sector and the readiness to adjust instruments to ensure price stability, all of which lean towards a hawkish outlook.</t>
         </is>
       </c>
     </row>
@@ -910,7 +910,7 @@
       </c>
       <c r="G13" t="inlineStr">
         <is>
-          <t>The article strongly supports combating inflation by raising interest rates significantly and maintaining them at restrictive levels. The emphasis on dampening demand to reduce inflation and the intention to continue raising interest rates in the future indicate a hawkish stance.</t>
+          <t>The article suggests a hawkish stance by indicating the intention of raising interest rates significantly and keeping them at restrictive levels to combat inflation. The Governing Council aims to reduce inflation by dampening demand and guard against the risk of persistent increase in inflation expectations, which are typical hawkish policies. Additionally, the decision to reduce the Eurosystem's holdings of securities under the asset purchase programme also reflects a hawkish tone towards monetary policy. The overall tone is focused on combating inflation and maintaining price stability.</t>
         </is>
       </c>
     </row>
@@ -942,12 +942,12 @@
       </c>
       <c r="F14" t="inlineStr">
         <is>
-          <t>0.9</t>
+          <t>0.8</t>
         </is>
       </c>
       <c r="G14" t="inlineStr">
         <is>
-          <t>The article is strongly hawkish as it indicates a significant increase in interest rates, with expectations of further increases to combat high inflation levels. The focus on the need for restrictive interest rate levels to reduce inflationary pressures and the projection of continued inflation above target levels contribute to the hawkish stance. Additionally, the planned reduction in asset purchases and discussion of normalizing monetary policy further support a hawkish outlook.</t>
+          <t>The article suggests a hawkish stance as it highlights the decision to raise interest rates significantly to combat high inflation levels. The Governing Council expects to continue raising rates in a steady manner to reach restrictive levels. Additionally, the article mentions a decline in the asset purchase program and a focus on reducing inflation, which align with a hawkish monetary policy stance aimed at controlling rising prices.</t>
         </is>
       </c>
     </row>
@@ -984,7 +984,7 @@
       </c>
       <c r="G15" t="inlineStr">
         <is>
-          <t>The article suggests a hawkish stance by emphasizing multiple increases in interest rates to combat high inflation, raising concerns about inflation remaining above target, and recalibrating monetary policy instruments to normalize conditions. The focus on inflation containment and gradual policy normalization indicates a hawkish monetary policy stance.</t>
+          <t>The article clearly indicates a hawkish stance as the ECB has decided to raise interest rates by a significant amount, recognizing high inflation levels as a major concern. The emphasis on normalizing monetary policy to combat rising inflation pressures and the commitment to adjusting all instruments within its mandate to stabilize inflation at the 2% target suggest a hawkish tone. The score of 0.8 reflects the strong hawkish sentiment conveyed in the article.</t>
         </is>
       </c>
     </row>
@@ -1021,7 +1021,7 @@
       </c>
       <c r="G16" t="inlineStr">
         <is>
-          <t>The article clearly indicates a hawkish stance by the Governing Council of the ECB. The decision to raise interest rates by a significant amount, the emphasis on combatting high inflation, and the adjustment of monetary policy instruments all point towards a hawkish outlook. The language used suggests a commitment to controlling inflation and normalizing monetary policy to address the rising inflationary pressures in the economy.</t>
+          <t>The article suggests a hawkish stance as it describes the European Central Bank's decision to raise interest rates multiple times to combat high inflation, with a focus on returning inflation to its 2% target. The emphasis on reducing support for demand, adjusting interest rates, and normalizing the monetary policy reflects a hawkish outlook towards controlling inflationary pressures.</t>
         </is>
       </c>
     </row>
@@ -1053,12 +1053,12 @@
       </c>
       <c r="F17" t="inlineStr">
         <is>
-          <t>0.9</t>
+          <t>0.8</t>
         </is>
       </c>
       <c r="G17" t="inlineStr">
         <is>
-          <t>The article suggests a hawkish stance by indicating a series of interest rate hikes to combat high inflation. The expectation is to raise interest rates further to dampen demand and guard against persistent inflation. This suggests a strong focus on combating inflation rather than supporting economic growth and low interest rates.</t>
+          <t>The article strongly indicates a hawkish stance by the ECB as it mentions the decision to raise interest rates significantly to combat high inflation levels. The emphasis on further interest rate hikes and the expectation for inflation to remain above target for an extended period all point towards a hawkish outlook. Additionally, the lowered economic growth projections and concerns about geopolitical situations further support the hawkish classification.</t>
         </is>
       </c>
     </row>
@@ -1085,17 +1085,17 @@
       </c>
       <c r="E18" t="inlineStr">
         <is>
-          <t>Hawkish</t>
+          <t>Error</t>
         </is>
       </c>
       <c r="F18" t="inlineStr">
         <is>
-          <t>0.9</t>
+          <t>Error</t>
         </is>
       </c>
       <c r="G18" t="inlineStr">
         <is>
-          <t>The article indicates a strong hawkish tone as the European Central Bank (ECB) is raising interest rates to combat high inflation. The ECB is taking steps to dampen demand and guard against persistent inflation pressures. There are clear mentions of the need to raise rates further and the expectation that inflation will remain above target for an extended period. Additionally, the article highlights concerns about rising inflation expectations, strong price pressures, and revised upward inflation projections. Overall, the emphasis is on combating inflation and maintaining price stability rather than focusing on economic growth or easing policies.</t>
+          <t>Error</t>
         </is>
       </c>
     </row>
@@ -1122,17 +1122,17 @@
       </c>
       <c r="E19" t="inlineStr">
         <is>
-          <t>Hawkish</t>
+          <t>Error</t>
         </is>
       </c>
       <c r="F19" t="inlineStr">
         <is>
-          <t>0.9</t>
+          <t>Error</t>
         </is>
       </c>
       <c r="G19" t="inlineStr">
         <is>
-          <t>The article indicates a hawkish stance as it mentions the Governing Council's commitment to price stability by raising interest rates and implementing the Transmission Protection Instrument (TPI) to support the effective transmission of monetary policy. The increased interest rates, future normalization plans, and emphasis on anchoring inflation expectations all point towards a hawkish monetary policy stance aimed at combating inflation and ensuring inflation returns to the 2% target over the medium term.</t>
+          <t>Error</t>
         </is>
       </c>
     </row>
@@ -1169,7 +1169,7 @@
       </c>
       <c r="G20" t="inlineStr">
         <is>
-          <t>The article suggests a hawkish stance by emphasizing the Governing Council's commitment to price stability and their decision to raise interest rates by 50 basis points. This indicates a focus on combating inflation and monetary tightening to ensure inflation returns to the 2% target over the medium term. The mention of normalizing monetary policy, frontloading the exit from negative interest rates, and the importance of the Transmission Protection Instrument (TPI) all lean towards a hawkish outlook.</t>
+          <t>The article suggests a hawkish stance by detailing the Governing Council's decision to raise interest rates significantly, implement the Transmission Protection Instrument (TPI) to support monetary policy transmission, and signal further normalization of interest rates in the future. These actions are aimed at combating inflation and ensuring price stability in the medium term.</t>
         </is>
       </c>
     </row>
@@ -1201,12 +1201,12 @@
       </c>
       <c r="F21" t="inlineStr">
         <is>
-          <t>0.9</t>
+          <t>0.8</t>
         </is>
       </c>
       <c r="G21" t="inlineStr">
         <is>
-          <t>The article indicates a hawkish stance by emphasizing the challenges of high inflation and the need to ensure it returns to the 2% target over the medium term. It mentions plans to raise interest rates and end asset purchases as part of normalizing monetary policy. The focus on combating inflation and the planned interest rate hikes signal a hawkish tone.</t>
+          <t>The article indicates a hawkish stance by discussing the challenges of high inflation and the measures being taken to combat it, such as raising interest rates and ending net asset purchases. The planned rate hikes and commitment to maintaining price stability signal a hawkish approach towards monetary policy.</t>
         </is>
       </c>
     </row>
@@ -1233,17 +1233,17 @@
       </c>
       <c r="E22" t="inlineStr">
         <is>
-          <t>Hawkish</t>
+          <t>Dovish</t>
         </is>
       </c>
       <c r="F22" t="inlineStr">
         <is>
-          <t>0.5</t>
+          <t>-0.7</t>
         </is>
       </c>
       <c r="G22" t="inlineStr">
         <is>
-          <t>The article suggests concerns about inflation pressures and acknowledges the need for eventual monetary policy tightening to combat high inflation. The mention of maintaining price stability at 2% and gradual adjustments to key ECB interest rates indicate a cautious approach towards controlling inflation, which leans towards a hawkish stance.</t>
+          <t>The article suggests that the economy is facing challenges due to the conflict in Ukraine and the associated uncertainties. It highlights that economic activity is still being supported by the reopening after the pandemic crisis, but inflation has increased significantly mainly due to rising energy costs. The European Central Bank (ECB) is maintaining a flexible approach to monetary policy, with a focus on price stability. The overall tone leans towards dovishness as the ECB is prepared to adjust its policies as needed to support economic recovery and ensure price stability.</t>
         </is>
       </c>
     </row>
@@ -1292,12 +1292,12 @@
       </c>
       <c r="F23" t="inlineStr">
         <is>
-          <t>-0.7</t>
+          <t>-0.5</t>
         </is>
       </c>
       <c r="G23" t="inlineStr">
         <is>
-          <t>The article suggests a dovish stance by mentioning the Governing Council's commitment to ensuring smooth liquidity conditions, supporting the people of Ukraine, and implementing measures to pursue price stability and safeguard financial stability. The revision of the asset purchase programme and continued reinvestment of principal payments also indicate a dovish tone. Overall, the emphasis on flexibility in monetary policy and readiness to adjust instruments as needed to stabilize inflation at 2% contribute to a dovish outlook.</t>
+          <t>The article suggests a dovish stance by emphasizing support for liquidity conditions, implementing sanctions for stability, and adjusting asset purchase programs to address the uncertain economic environment. The ECB maintains a commitment to maintaining accommodative monetary policy and supporting economic recovery. The dovish score of -0.5 reflects a moderately supportive tone towards economic growth and price stability.</t>
         </is>
       </c>
     </row>
@@ -1349,7 +1349,7 @@
       </c>
       <c r="G24" t="inlineStr">
         <is>
-          <t>The article suggests a dovish stance with continued accommodative monetary policy measures, including maintaining low interest rates, continuing asset purchases, and reinvesting principal payments to maintain monetary accommodation. The intention to adjust all instruments as necessary to ensure inflation stabilizes at the 2% target over the medium term further supports the dovish outlook. However, the gradual reduction in asset purchases under the APP indicates a slight hawkish tone, reflected in the negative score.</t>
+          <t>The article suggests a dovish stance by detailing the continuation of asset purchase programs, the maintenance of low interest rates, and the commitment to maintaining accommodative monetary policy until inflation reaches the target of 2%. The flexibility and reinforcement of asset purchases indicate a supportive approach to economic growth and price stability. The score is closer to -1, indicating a strongly dovish sentiment.</t>
         </is>
       </c>
     </row>
@@ -1396,12 +1396,12 @@
       </c>
       <c r="F25" t="inlineStr">
         <is>
-          <t>0.7</t>
+          <t>0.6</t>
         </is>
       </c>
       <c r="G25" t="inlineStr">
         <is>
-          <t>The article suggests a gradual reduction in asset purchases and a commitment to maintaining accommodative monetary policy until inflation stabilizes at the 2% target over the medium term. The decision to adjust asset purchases and maintain an accommodative stance shows a hawkish stance towards potential inflationary pressures.</t>
+          <t>The article suggests a hawkish stance by outlining a reduction in asset purchases, maintaining accommodative monetary policy, and signaling a possible increase in interest rates in the future. The Governing Council's focus on inflation reaching and stabilizing at 2% and the intention to adjust instruments to ensure this target indicates a hawkish bias towards combating inflation.</t>
         </is>
       </c>
     </row>
@@ -1450,12 +1450,12 @@
       </c>
       <c r="F26" t="inlineStr">
         <is>
-          <t>-0.6</t>
+          <t>-0.8</t>
         </is>
       </c>
       <c r="G26" t="inlineStr">
         <is>
-          <t>The article suggests a continuation of accommodative monetary policies to support economic growth and inflation. The focus on maintaining favorable financing conditions, the commitment to low-interest rates, and the extension of asset purchase programs all indicate dovishness.</t>
+          <t>The article suggests a dovish stance as it emphasizes maintaining accommodative monetary policy measures to support economic recovery and achieve the inflation target of two per cent over the medium term. The continuation of net asset purchases under the PEPP, the unchanged interest rates, and the commitment to provide ample liquidity all reflect a supportive stance towards economic growth and low-interest rates.</t>
         </is>
       </c>
     </row>
@@ -1509,7 +1509,7 @@
       </c>
       <c r="G27" t="inlineStr">
         <is>
-          <t>The article suggests dovish sentiments as the Governing Council of the European Central Bank (ECB) announces to maintain favourable financing conditions with a moderately lower pace of net asset purchases under the pandemic emergency purchase programme. The decision to continue net purchases under the asset purchase programme (APP) and reinvesting principal payments from maturing securities purchased under both the APP and the pandemic emergency purchase programme (PEPP) indicates a supportive stance towards economic growth and monetary easing. The commitment to keep key ECB interest rates at low levels until inflation reaches two per cent and to provide ample liquidity through refinancing operations further align with dovish policies. Although there is acknowledgment of the symmetric two per cent</t>
+          <t>The article suggests a continuation of accommodative monetary policy measures such as maintaining low interest rates, ongoing asset purchases, and ensuring ample liquidity in the financial system. The focus is on supporting the economy and maintaining favorable financing conditions, indicating a dovish stance overall. The score is slightly below neutral indicating a modestly dovish sentiment.</t>
         </is>
       </c>
     </row>
@@ -1565,7 +1565,7 @@
       </c>
       <c r="G28" t="inlineStr">
         <is>
-          <t>The article is dovish as it emphasizes the commitment of the Governing Council to maintain an accommodative monetary policy stance to meet its inflation target. The symmetric two per cent inflation target and the intention to keep interest rates low until inflation reaches the target suggest a dovish stance. Additionally, the continuation of asset purchase programs and reinvestment policies further support the dovish outlook.</t>
+          <t>The article suggests a highly dovish stance as the European Central Bank (ECB) is committed to maintaining an accommodative monetary policy stance to meet its inflation target of two per cent. The ECB plans to keep interest rates low until inflation reaches the target well ahead of the projection horizon. The article also outlines continued asset purchases and liquidity provision measures to support economic recovery and price stability.</t>
         </is>
       </c>
     </row>
@@ -1611,7 +1611,7 @@
       </c>
       <c r="G29" t="inlineStr">
         <is>
-          <t>The article suggests a very accommodative monetary policy stance aimed at supporting economic growth and countering the negative impact of the pandemic on inflation. The continuation of net asset purchases, reinvestment of principal payments, and providing ample liquidity all signal a dovish approach towards maintaining favorable financing conditions and supporting the smooth transmission of monetary policy. The commitment to adjusting instruments as necessary to ensure inflation moves towards the target in a sustained manner further emphasizes a dovish stance.</t>
+          <t>The article highlights a very accommodative monetary policy stance with unchanged low interest rates, continued net asset purchases, and a commitment to provide ample liquidity. The focus on supporting financing conditions and countering the downward impact of the pandemic on inflation suggests a dovish stance aimed at fostering economic growth and maintaining low interest rates.</t>
         </is>
       </c>
     </row>
@@ -1657,7 +1657,7 @@
       </c>
       <c r="G30" t="inlineStr">
         <is>
-          <t>The article is classified as dovish because it emphasizes maintaining an accommodative monetary policy stance to support economic recovery and counter the negative impact of the pandemic on inflation. The continued commitment to low interest rates, asset purchases, and ample liquidity provision indicates a dovish sentiment towards promoting economic growth. The score of -0.8 suggests a strong leaning towards dovish policies.</t>
+          <t>The article suggests a highly accommodative monetary policy stance by keeping interest rates at historic lows and continuing with net asset purchases. The emphasis on maintaining favorable financing conditions and supporting the smooth transmission of monetary policy indicate a dovish stance aimed at countering the negative impact of the pandemic on inflation and economic growth. The commitment to adjusting all instruments as necessary to ensure inflation moves towards the target in a sustained manner also reflects a dovish predisposition.</t>
         </is>
       </c>
     </row>
@@ -1703,7 +1703,7 @@
       </c>
       <c r="G31" t="inlineStr">
         <is>
-          <t>The article indicates a dovish stance by emphasizing continued asset purchases, reinvestment of principal payments, and maintaining low interest rates. The primary focus is on supporting economic recovery and countering the negative impact of the pandemic on inflation, demonstrating a dovish policy stance.</t>
+          <t>The article suggests a dovish stance by indicating continued net asset purchases, maintaining low interest rates, and providing ample liquidity. The emphasis on flexibility in asset purchases and the commitment to maintaining accommodative policies until inflation reaches the desired level all point towards supportive measures for economic growth. The score of -0.8 reflects a moderately dovish stance.</t>
         </is>
       </c>
     </row>
@@ -1748,7 +1748,7 @@
       </c>
       <c r="G32" t="inlineStr">
         <is>
-          <t>The article indicates a very accommodative monetary policy stance with low interest rates, continued asset purchases, and ample liquidity provision. The focus on maintaining favorable financing conditions and supporting economic recovery suggests a dovish stance aimed at fostering growth rather than combatting inflation. The score of -0.9 indicates a strong dovish leaning.</t>
+          <t>The article suggests a very accommodative monetary policy stance with a focus on supporting economic growth and maintaining low interest rates. The continuation of asset purchases and reinvestment of principal payments indicate a commitment to providing ample liquidity and monetary accommodation. The language used in the article leans heavily towards dovish policies aimed at bolstering the economy and ensuring inflation converges to target levels.</t>
         </is>
       </c>
     </row>

</xml_diff>